<commit_message>
one coordinate error for a rogue Churchill Mesic 1 specimen
</commit_message>
<xml_diff>
--- a/Data/Inventory of Specimens.xlsx
+++ b/Data/Inventory of Specimens.xlsx
@@ -1,8 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{38C2C22D-D124-4D8C-A226-33E8070C9B6E}" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{D13ACAA2-9465-4CF9-BB28-505BD326B5EF}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3749,8 +3750,8 @@
   <dimension ref="A1:N1449"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1420" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N1436" sqref="N1436"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I87" sqref="I87:J87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7457,16 +7458,16 @@
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A87" s="18" t="s">
-        <v>37</v>
+      <c r="A87" s="26" t="s">
+        <v>560</v>
       </c>
       <c r="B87" s="25" t="s">
-        <v>38</v>
+        <v>624</v>
       </c>
       <c r="C87" s="25" t="s">
-        <v>331</v>
-      </c>
-      <c r="D87" s="26">
+        <v>627</v>
+      </c>
+      <c r="D87" s="18">
         <v>1</v>
       </c>
       <c r="E87" s="18" t="s">
@@ -7482,35 +7483,29 @@
         <v>770</v>
       </c>
       <c r="I87" s="30">
-        <v>58.732349999999997</v>
+        <v>58.733510000000003</v>
       </c>
       <c r="J87" s="30">
-        <v>-93.790279999999996</v>
+        <v>-93.797920000000005</v>
       </c>
       <c r="K87" s="18" t="s">
         <v>16</v>
       </c>
       <c r="L87" s="18">
-        <v>2</v>
-      </c>
-      <c r="M87" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="N87" s="18" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="18" t="s">
-        <v>89</v>
+        <v>37</v>
       </c>
       <c r="B88" s="25" t="s">
-        <v>92</v>
+        <v>38</v>
       </c>
       <c r="C88" s="25" t="s">
-        <v>356</v>
-      </c>
-      <c r="D88" s="18">
+        <v>331</v>
+      </c>
+      <c r="D88" s="26">
         <v>1</v>
       </c>
       <c r="E88" s="18" t="s">
@@ -7552,7 +7547,7 @@
         <v>92</v>
       </c>
       <c r="C89" s="25" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D89" s="18">
         <v>1</v>
@@ -7590,16 +7585,16 @@
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="18" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B90" s="25" t="s">
-        <v>133</v>
+        <v>92</v>
       </c>
       <c r="C90" s="25" t="s">
-        <v>414</v>
+        <v>357</v>
       </c>
       <c r="D90" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E90" s="18" t="s">
         <v>51</v>
@@ -7634,16 +7629,16 @@
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="18" t="s">
-        <v>227</v>
+        <v>98</v>
       </c>
       <c r="B91" s="25" t="s">
-        <v>247</v>
+        <v>133</v>
       </c>
       <c r="C91" s="25" t="s">
-        <v>527</v>
+        <v>414</v>
       </c>
       <c r="D91" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E91" s="18" t="s">
         <v>51</v>
@@ -7681,10 +7676,10 @@
         <v>227</v>
       </c>
       <c r="B92" s="25" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C92" s="25" t="s">
-        <v>549</v>
+        <v>527</v>
       </c>
       <c r="D92" s="18">
         <v>1</v>
@@ -7722,16 +7717,16 @@
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="18" t="s">
-        <v>56</v>
+        <v>227</v>
       </c>
       <c r="B93" s="25" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="C93" s="25" t="s">
-        <v>346</v>
+        <v>549</v>
       </c>
       <c r="D93" s="18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E93" s="18" t="s">
         <v>51</v>
@@ -7761,7 +7756,7 @@
         <v>126</v>
       </c>
       <c r="N93" s="18" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
@@ -7775,7 +7770,7 @@
         <v>346</v>
       </c>
       <c r="D94" s="18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E94" s="18" t="s">
         <v>51</v>
@@ -7802,21 +7797,21 @@
         <v>2</v>
       </c>
       <c r="M94" s="18" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="N94" s="18" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="18" t="s">
-        <v>98</v>
+        <v>56</v>
       </c>
       <c r="B95" s="25" t="s">
-        <v>133</v>
+        <v>267</v>
       </c>
       <c r="C95" s="25" t="s">
-        <v>415</v>
+        <v>346</v>
       </c>
       <c r="D95" s="18">
         <v>1</v>
@@ -7853,22 +7848,22 @@
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A96" s="28" t="s">
-        <v>227</v>
-      </c>
-      <c r="B96" s="31" t="s">
-        <v>247</v>
-      </c>
-      <c r="C96" s="31" t="s">
-        <v>528</v>
-      </c>
-      <c r="D96" s="28">
-        <v>1</v>
-      </c>
-      <c r="E96" s="28" t="s">
+      <c r="A96" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B96" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="C96" s="25" t="s">
+        <v>415</v>
+      </c>
+      <c r="D96" s="18">
+        <v>1</v>
+      </c>
+      <c r="E96" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="F96" s="28" t="s">
+      <c r="F96" s="26" t="s">
         <v>52</v>
       </c>
       <c r="G96" s="18" t="s">
@@ -7877,34 +7872,34 @@
       <c r="H96" s="18" t="s">
         <v>770</v>
       </c>
-      <c r="I96" s="29">
+      <c r="I96" s="30">
         <v>58.732349999999997</v>
       </c>
-      <c r="J96" s="29">
+      <c r="J96" s="30">
         <v>-93.790279999999996</v>
       </c>
       <c r="K96" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="L96" s="28">
-        <v>2</v>
-      </c>
-      <c r="M96" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="N96" s="28" t="s">
-        <v>68</v>
+      <c r="L96" s="18">
+        <v>2</v>
+      </c>
+      <c r="M96" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="N96" s="18" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="28" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="B97" s="31" t="s">
-        <v>224</v>
+        <v>247</v>
       </c>
       <c r="C97" s="31" t="s">
-        <v>503</v>
+        <v>528</v>
       </c>
       <c r="D97" s="28">
         <v>1</v>
@@ -7934,29 +7929,29 @@
         <v>2</v>
       </c>
       <c r="M97" s="28" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="N97" s="28" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A98" s="26" t="s">
-        <v>560</v>
-      </c>
-      <c r="B98" s="25" t="s">
-        <v>598</v>
-      </c>
-      <c r="C98" s="25" t="s">
-        <v>599</v>
-      </c>
-      <c r="D98" s="18">
-        <v>3</v>
-      </c>
-      <c r="E98" s="18" t="s">
+      <c r="A98" s="28" t="s">
+        <v>219</v>
+      </c>
+      <c r="B98" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="C98" s="31" t="s">
+        <v>503</v>
+      </c>
+      <c r="D98" s="28">
+        <v>1</v>
+      </c>
+      <c r="E98" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="F98" s="26" t="s">
+      <c r="F98" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G98" s="18" t="s">
@@ -7965,17 +7960,23 @@
       <c r="H98" s="18" t="s">
         <v>770</v>
       </c>
-      <c r="I98" s="30">
+      <c r="I98" s="29">
         <v>58.732349999999997</v>
       </c>
-      <c r="J98" s="30">
+      <c r="J98" s="29">
         <v>-93.790279999999996</v>
       </c>
       <c r="K98" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="L98" s="18">
-        <v>2</v>
+      <c r="L98" s="28">
+        <v>2</v>
+      </c>
+      <c r="M98" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="N98" s="28" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.25">
@@ -7983,13 +7984,13 @@
         <v>560</v>
       </c>
       <c r="B99" s="25" t="s">
-        <v>615</v>
+        <v>598</v>
       </c>
       <c r="C99" s="25" t="s">
-        <v>614</v>
+        <v>599</v>
       </c>
       <c r="D99" s="18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E99" s="18" t="s">
         <v>51</v>
@@ -8021,10 +8022,10 @@
         <v>560</v>
       </c>
       <c r="B100" s="25" t="s">
-        <v>624</v>
+        <v>615</v>
       </c>
       <c r="C100" s="25" t="s">
-        <v>626</v>
+        <v>614</v>
       </c>
       <c r="D100" s="18">
         <v>1</v>
@@ -8062,7 +8063,7 @@
         <v>624</v>
       </c>
       <c r="C101" s="25" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D101" s="18">
         <v>1</v>
@@ -8100,7 +8101,7 @@
         <v>624</v>
       </c>
       <c r="C102" s="25" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D102" s="18">
         <v>1</v>
@@ -8135,10 +8136,10 @@
         <v>560</v>
       </c>
       <c r="B103" s="25" t="s">
-        <v>647</v>
+        <v>624</v>
       </c>
       <c r="C103" s="25" t="s">
-        <v>649</v>
+        <v>628</v>
       </c>
       <c r="D103" s="18">
         <v>1</v>
@@ -8169,16 +8170,16 @@
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A104" s="20" t="s">
-        <v>208</v>
+      <c r="A104" s="26" t="s">
+        <v>560</v>
       </c>
       <c r="B104" s="25" t="s">
-        <v>689</v>
+        <v>647</v>
       </c>
       <c r="C104" s="25" t="s">
-        <v>693</v>
-      </c>
-      <c r="D104" s="24">
+        <v>649</v>
+      </c>
+      <c r="D104" s="18">
         <v>1</v>
       </c>
       <c r="E104" s="18" t="s">
@@ -8202,7 +8203,7 @@
       <c r="K104" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="L104" s="23">
+      <c r="L104" s="18">
         <v>2</v>
       </c>
     </row>
@@ -8211,10 +8212,10 @@
         <v>208</v>
       </c>
       <c r="B105" s="25" t="s">
-        <v>701</v>
+        <v>689</v>
       </c>
       <c r="C105" s="25" t="s">
-        <v>707</v>
+        <v>693</v>
       </c>
       <c r="D105" s="24">
         <v>1</v>
@@ -8245,16 +8246,16 @@
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A106" s="18" t="s">
-        <v>37</v>
+      <c r="A106" s="20" t="s">
+        <v>208</v>
       </c>
       <c r="B106" s="25" t="s">
-        <v>38</v>
+        <v>701</v>
       </c>
       <c r="C106" s="25" t="s">
-        <v>328</v>
-      </c>
-      <c r="D106" s="26">
+        <v>707</v>
+      </c>
+      <c r="D106" s="24">
         <v>1</v>
       </c>
       <c r="E106" s="18" t="s">
@@ -8270,35 +8271,29 @@
         <v>770</v>
       </c>
       <c r="I106" s="30">
-        <v>58.722349999999999</v>
+        <v>58.732349999999997</v>
       </c>
       <c r="J106" s="30">
-        <v>-93.839910000000003</v>
+        <v>-93.790279999999996</v>
       </c>
       <c r="K106" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="L106" s="18">
-        <v>3</v>
-      </c>
-      <c r="M106" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="N106" s="18" t="s">
-        <v>12</v>
+      <c r="L106" s="23">
+        <v>2</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" s="18" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="B107" s="25" t="s">
-        <v>138</v>
+        <v>38</v>
       </c>
       <c r="C107" s="25" t="s">
-        <v>419</v>
-      </c>
-      <c r="D107" s="18">
+        <v>328</v>
+      </c>
+      <c r="D107" s="26">
         <v>1</v>
       </c>
       <c r="E107" s="18" t="s">
@@ -8340,7 +8335,7 @@
         <v>138</v>
       </c>
       <c r="C108" s="25" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="D108" s="18">
         <v>1</v>
@@ -8378,13 +8373,13 @@
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" s="18" t="s">
-        <v>149</v>
+        <v>98</v>
       </c>
       <c r="B109" s="25" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="C109" s="25" t="s">
-        <v>436</v>
+        <v>422</v>
       </c>
       <c r="D109" s="18">
         <v>1</v>
@@ -8422,13 +8417,13 @@
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" s="18" t="s">
-        <v>219</v>
+        <v>149</v>
       </c>
       <c r="B110" s="25" t="s">
-        <v>223</v>
+        <v>154</v>
       </c>
       <c r="C110" s="25" t="s">
-        <v>488</v>
+        <v>436</v>
       </c>
       <c r="D110" s="18">
         <v>1</v>
@@ -8466,13 +8461,13 @@
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" s="18" t="s">
-        <v>98</v>
+        <v>219</v>
       </c>
       <c r="B111" s="25" t="s">
-        <v>101</v>
+        <v>223</v>
       </c>
       <c r="C111" s="25" t="s">
-        <v>404</v>
+        <v>488</v>
       </c>
       <c r="D111" s="18">
         <v>1</v>
@@ -8502,7 +8497,7 @@
         <v>3</v>
       </c>
       <c r="M111" s="18" t="s">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="N111" s="18" t="s">
         <v>12</v>
@@ -8513,13 +8508,13 @@
         <v>98</v>
       </c>
       <c r="B112" s="25" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="C112" s="25" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D112" s="18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E112" s="18" t="s">
         <v>51</v>
@@ -8554,16 +8549,16 @@
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A113" s="18" t="s">
-        <v>56</v>
+        <v>98</v>
       </c>
       <c r="B113" s="25" t="s">
-        <v>265</v>
+        <v>117</v>
       </c>
       <c r="C113" s="25" t="s">
-        <v>345</v>
+        <v>408</v>
       </c>
       <c r="D113" s="18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E113" s="18" t="s">
         <v>51</v>
@@ -8590,29 +8585,29 @@
         <v>3</v>
       </c>
       <c r="M113" s="18" t="s">
-        <v>130</v>
+        <v>103</v>
       </c>
       <c r="N113" s="18" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A114" s="28" t="s">
-        <v>219</v>
-      </c>
-      <c r="B114" s="31" t="s">
-        <v>224</v>
-      </c>
-      <c r="C114" s="31" t="s">
-        <v>503</v>
-      </c>
-      <c r="D114" s="28">
-        <v>1</v>
-      </c>
-      <c r="E114" s="28" t="s">
+      <c r="A114" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B114" s="25" t="s">
+        <v>265</v>
+      </c>
+      <c r="C114" s="25" t="s">
+        <v>345</v>
+      </c>
+      <c r="D114" s="18">
+        <v>1</v>
+      </c>
+      <c r="E114" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="F114" s="28" t="s">
+      <c r="F114" s="26" t="s">
         <v>52</v>
       </c>
       <c r="G114" s="18" t="s">
@@ -8621,37 +8616,37 @@
       <c r="H114" s="18" t="s">
         <v>770</v>
       </c>
-      <c r="I114" s="29">
+      <c r="I114" s="30">
         <v>58.722349999999999</v>
       </c>
-      <c r="J114" s="29">
+      <c r="J114" s="30">
         <v>-93.839910000000003</v>
       </c>
       <c r="K114" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="L114" s="28">
+      <c r="L114" s="18">
         <v>3</v>
       </c>
-      <c r="M114" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="N114" s="28" t="s">
-        <v>68</v>
+      <c r="M114" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="N114" s="18" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115" s="28" t="s">
-        <v>98</v>
+        <v>219</v>
       </c>
       <c r="B115" s="31" t="s">
-        <v>101</v>
+        <v>224</v>
       </c>
       <c r="C115" s="31" t="s">
-        <v>745</v>
+        <v>503</v>
       </c>
       <c r="D115" s="28">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E115" s="28" t="s">
         <v>51</v>
@@ -8678,29 +8673,29 @@
         <v>3</v>
       </c>
       <c r="M115" s="28" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
       <c r="N115" s="28" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A116" s="18" t="s">
-        <v>560</v>
-      </c>
-      <c r="B116" s="25" t="s">
-        <v>561</v>
-      </c>
-      <c r="C116" s="25" t="s">
-        <v>562</v>
-      </c>
-      <c r="D116" s="18">
-        <v>1</v>
-      </c>
-      <c r="E116" s="18" t="s">
+      <c r="A116" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B116" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="C116" s="31" t="s">
+        <v>745</v>
+      </c>
+      <c r="D116" s="28">
+        <v>3</v>
+      </c>
+      <c r="E116" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="F116" s="26" t="s">
+      <c r="F116" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G116" s="18" t="s">
@@ -8709,17 +8704,23 @@
       <c r="H116" s="18" t="s">
         <v>770</v>
       </c>
-      <c r="I116" s="30">
+      <c r="I116" s="29">
         <v>58.722349999999999</v>
       </c>
-      <c r="J116" s="30">
+      <c r="J116" s="29">
         <v>-93.839910000000003</v>
       </c>
       <c r="K116" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="L116" s="18">
+      <c r="L116" s="28">
         <v>3</v>
+      </c>
+      <c r="M116" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="N116" s="28" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.25">
@@ -8727,10 +8728,10 @@
         <v>560</v>
       </c>
       <c r="B117" s="25" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C117" s="25" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="D117" s="18">
         <v>1</v>
@@ -8761,14 +8762,14 @@
       </c>
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A118" s="26" t="s">
+      <c r="A118" s="18" t="s">
         <v>560</v>
       </c>
       <c r="B118" s="25" t="s">
-        <v>606</v>
+        <v>563</v>
       </c>
       <c r="C118" s="25" t="s">
-        <v>607</v>
+        <v>565</v>
       </c>
       <c r="D118" s="18">
         <v>1</v>
@@ -8803,13 +8804,13 @@
         <v>560</v>
       </c>
       <c r="B119" s="25" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="C119" s="25" t="s">
-        <v>614</v>
+        <v>607</v>
       </c>
       <c r="D119" s="18">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E119" s="18" t="s">
         <v>51</v>
@@ -8844,10 +8845,10 @@
         <v>615</v>
       </c>
       <c r="C120" s="25" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="D120" s="18">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E120" s="18" t="s">
         <v>51</v>
@@ -8879,10 +8880,10 @@
         <v>560</v>
       </c>
       <c r="B121" s="25" t="s">
-        <v>624</v>
+        <v>615</v>
       </c>
       <c r="C121" s="25" t="s">
-        <v>626</v>
+        <v>617</v>
       </c>
       <c r="D121" s="18">
         <v>1</v>
@@ -8920,7 +8921,7 @@
         <v>624</v>
       </c>
       <c r="C122" s="25" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D122" s="18">
         <v>1</v>
@@ -8955,10 +8956,10 @@
         <v>560</v>
       </c>
       <c r="B123" s="25" t="s">
-        <v>639</v>
+        <v>624</v>
       </c>
       <c r="C123" s="25" t="s">
-        <v>642</v>
+        <v>627</v>
       </c>
       <c r="D123" s="18">
         <v>1</v>
@@ -8993,13 +8994,13 @@
         <v>560</v>
       </c>
       <c r="B124" s="25" t="s">
-        <v>647</v>
+        <v>639</v>
       </c>
       <c r="C124" s="25" t="s">
-        <v>651</v>
+        <v>642</v>
       </c>
       <c r="D124" s="18">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E124" s="18" t="s">
         <v>51</v>
@@ -9031,13 +9032,13 @@
         <v>560</v>
       </c>
       <c r="B125" s="25" t="s">
-        <v>624</v>
+        <v>647</v>
       </c>
       <c r="C125" s="25" t="s">
-        <v>627</v>
+        <v>651</v>
       </c>
       <c r="D125" s="18">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E125" s="18" t="s">
         <v>51</v>
@@ -9061,7 +9062,7 @@
         <v>16</v>
       </c>
       <c r="L125" s="18">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.25">
@@ -24259,17 +24260,17 @@
       </c>
     </row>
     <row r="484" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A484" s="18" t="s">
-        <v>10</v>
+      <c r="A484" s="26" t="s">
+        <v>560</v>
       </c>
       <c r="B484" s="25" t="s">
-        <v>11</v>
+        <v>615</v>
       </c>
       <c r="C484" s="25" t="s">
-        <v>291</v>
+        <v>616</v>
       </c>
       <c r="D484" s="18">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E484" s="18" t="s">
         <v>13</v>
@@ -24284,22 +24285,16 @@
         <v>770</v>
       </c>
       <c r="I484" s="30">
-        <v>51.244660000000003</v>
+        <v>51.246220000000001</v>
       </c>
       <c r="J484" s="30">
-        <v>-80.677670000000006</v>
+        <v>-80.672809999999998</v>
       </c>
       <c r="K484" s="18" t="s">
         <v>16</v>
       </c>
       <c r="L484" s="18">
-        <v>2</v>
-      </c>
-      <c r="M484" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="N484" s="18" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="485" spans="1:14" x14ac:dyDescent="0.25">
@@ -24307,13 +24302,13 @@
         <v>10</v>
       </c>
       <c r="B485" s="25" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C485" s="25" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D485" s="18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E485" s="18" t="s">
         <v>13</v>
@@ -24348,15 +24343,15 @@
     </row>
     <row r="486" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A486" s="18" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="B486" s="25" t="s">
-        <v>259</v>
+        <v>24</v>
       </c>
       <c r="C486" s="25" t="s">
-        <v>300</v>
-      </c>
-      <c r="D486" s="26">
+        <v>294</v>
+      </c>
+      <c r="D486" s="18">
         <v>3</v>
       </c>
       <c r="E486" s="18" t="s">
@@ -24395,13 +24390,13 @@
         <v>37</v>
       </c>
       <c r="B487" s="25" t="s">
-        <v>41</v>
+        <v>259</v>
       </c>
       <c r="C487" s="25" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D487" s="26">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E487" s="18" t="s">
         <v>13</v>
@@ -24439,10 +24434,10 @@
         <v>37</v>
       </c>
       <c r="B488" s="25" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C488" s="25" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D488" s="26">
         <v>1</v>
@@ -24486,7 +24481,7 @@
         <v>38</v>
       </c>
       <c r="C489" s="25" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D489" s="26">
         <v>1</v>
@@ -24530,10 +24525,10 @@
         <v>38</v>
       </c>
       <c r="C490" s="25" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D490" s="26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E490" s="18" t="s">
         <v>13</v>
@@ -24574,10 +24569,10 @@
         <v>38</v>
       </c>
       <c r="C491" s="25" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D491" s="26">
-        <v>77</v>
+        <v>2</v>
       </c>
       <c r="E491" s="18" t="s">
         <v>13</v>
@@ -24618,10 +24613,10 @@
         <v>38</v>
       </c>
       <c r="C492" s="25" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D492" s="26">
-        <v>1</v>
+        <v>77</v>
       </c>
       <c r="E492" s="18" t="s">
         <v>13</v>
@@ -24662,7 +24657,7 @@
         <v>38</v>
       </c>
       <c r="C493" s="25" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D493" s="26">
         <v>1</v>
@@ -24706,10 +24701,10 @@
         <v>38</v>
       </c>
       <c r="C494" s="25" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D494" s="26">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E494" s="18" t="s">
         <v>13</v>
@@ -24750,10 +24745,10 @@
         <v>38</v>
       </c>
       <c r="C495" s="25" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D495" s="26">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E495" s="18" t="s">
         <v>13</v>
@@ -24794,7 +24789,7 @@
         <v>38</v>
       </c>
       <c r="C496" s="25" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D496" s="26">
         <v>2</v>
@@ -24838,10 +24833,10 @@
         <v>38</v>
       </c>
       <c r="C497" s="25" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D497" s="26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E497" s="18" t="s">
         <v>13</v>
@@ -24882,7 +24877,7 @@
         <v>38</v>
       </c>
       <c r="C498" s="25" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="D498" s="26">
         <v>1</v>
@@ -24926,7 +24921,7 @@
         <v>38</v>
       </c>
       <c r="C499" s="25" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D499" s="26">
         <v>1</v>
@@ -24970,7 +24965,7 @@
         <v>38</v>
       </c>
       <c r="C500" s="25" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D500" s="26">
         <v>1</v>
@@ -25008,15 +25003,15 @@
     </row>
     <row r="501" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A501" s="18" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="B501" s="25" t="s">
-        <v>80</v>
+        <v>38</v>
       </c>
       <c r="C501" s="25" t="s">
-        <v>349</v>
-      </c>
-      <c r="D501" s="18">
+        <v>335</v>
+      </c>
+      <c r="D501" s="26">
         <v>1</v>
       </c>
       <c r="E501" s="18" t="s">
@@ -25052,16 +25047,16 @@
     </row>
     <row r="502" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A502" s="18" t="s">
-        <v>98</v>
+        <v>57</v>
       </c>
       <c r="B502" s="25" t="s">
-        <v>138</v>
+        <v>80</v>
       </c>
       <c r="C502" s="25" t="s">
-        <v>424</v>
+        <v>349</v>
       </c>
       <c r="D502" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E502" s="18" t="s">
         <v>13</v>
@@ -25099,13 +25094,13 @@
         <v>98</v>
       </c>
       <c r="B503" s="25" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C503" s="25" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D503" s="18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E503" s="18" t="s">
         <v>13</v>
@@ -25140,16 +25135,16 @@
     </row>
     <row r="504" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A504" s="18" t="s">
-        <v>149</v>
+        <v>98</v>
       </c>
       <c r="B504" s="25" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C504" s="25" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D504" s="18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E504" s="18" t="s">
         <v>13</v>
@@ -25184,16 +25179,16 @@
     </row>
     <row r="505" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A505" s="18" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="B505" s="25" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C505" s="25" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="D505" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E505" s="18" t="s">
         <v>13</v>
@@ -25228,16 +25223,16 @@
     </row>
     <row r="506" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A506" s="18" t="s">
-        <v>185</v>
+        <v>159</v>
       </c>
       <c r="B506" s="25" t="s">
-        <v>186</v>
+        <v>160</v>
       </c>
       <c r="C506" s="25" t="s">
-        <v>453</v>
+        <v>438</v>
       </c>
       <c r="D506" s="18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E506" s="18" t="s">
         <v>13</v>
@@ -25272,16 +25267,16 @@
     </row>
     <row r="507" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A507" s="18" t="s">
-        <v>219</v>
+        <v>185</v>
       </c>
       <c r="B507" s="25" t="s">
-        <v>223</v>
+        <v>186</v>
       </c>
       <c r="C507" s="25" t="s">
-        <v>481</v>
+        <v>453</v>
       </c>
       <c r="D507" s="18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E507" s="18" t="s">
         <v>13</v>
@@ -25322,10 +25317,10 @@
         <v>223</v>
       </c>
       <c r="C508" s="25" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
       <c r="D508" s="18">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E508" s="18" t="s">
         <v>13</v>
@@ -25363,13 +25358,13 @@
         <v>219</v>
       </c>
       <c r="B509" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C509" s="25" t="s">
-        <v>501</v>
+        <v>488</v>
       </c>
       <c r="D509" s="18">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E509" s="18" t="s">
         <v>13</v>
@@ -25404,16 +25399,16 @@
     </row>
     <row r="510" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A510" s="18" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B510" s="25" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C510" s="25" t="s">
-        <v>515</v>
+        <v>501</v>
       </c>
       <c r="D510" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E510" s="18" t="s">
         <v>13</v>
@@ -25454,10 +25449,10 @@
         <v>228</v>
       </c>
       <c r="C511" s="25" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D511" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E511" s="18" t="s">
         <v>13</v>
@@ -25498,10 +25493,10 @@
         <v>228</v>
       </c>
       <c r="C512" s="25" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D512" s="18">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E512" s="18" t="s">
         <v>13</v>
@@ -25539,13 +25534,13 @@
         <v>227</v>
       </c>
       <c r="B513" s="25" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C513" s="25" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D513" s="18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E513" s="18" t="s">
         <v>13</v>
@@ -25586,10 +25581,10 @@
         <v>229</v>
       </c>
       <c r="C514" s="25" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D514" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E514" s="18" t="s">
         <v>13</v>
@@ -25627,13 +25622,13 @@
         <v>227</v>
       </c>
       <c r="B515" s="25" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C515" s="25" t="s">
-        <v>536</v>
+        <v>519</v>
       </c>
       <c r="D515" s="18">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="E515" s="18" t="s">
         <v>13</v>
@@ -25668,16 +25663,16 @@
     </row>
     <row r="516" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A516" s="18" t="s">
-        <v>98</v>
+        <v>227</v>
       </c>
       <c r="B516" s="25" t="s">
-        <v>144</v>
+        <v>236</v>
       </c>
       <c r="C516" s="25" t="s">
-        <v>374</v>
+        <v>536</v>
       </c>
       <c r="D516" s="18">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="E516" s="18" t="s">
         <v>13</v>
@@ -25704,7 +25699,7 @@
         <v>2</v>
       </c>
       <c r="M516" s="18" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N516" s="18" t="s">
         <v>12</v>
@@ -25712,13 +25707,13 @@
     </row>
     <row r="517" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A517" s="18" t="s">
-        <v>219</v>
+        <v>98</v>
       </c>
       <c r="B517" s="25" t="s">
-        <v>223</v>
+        <v>144</v>
       </c>
       <c r="C517" s="25" t="s">
-        <v>488</v>
+        <v>374</v>
       </c>
       <c r="D517" s="18">
         <v>1</v>
@@ -25756,13 +25751,13 @@
     </row>
     <row r="518" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A518" s="18" t="s">
-        <v>55</v>
+        <v>219</v>
       </c>
       <c r="B518" s="25" t="s">
-        <v>71</v>
+        <v>223</v>
       </c>
       <c r="C518" s="25" t="s">
-        <v>339</v>
+        <v>488</v>
       </c>
       <c r="D518" s="18">
         <v>1</v>
@@ -25792,7 +25787,7 @@
         <v>2</v>
       </c>
       <c r="M518" s="18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N518" s="18" t="s">
         <v>12</v>
@@ -25800,16 +25795,16 @@
     </row>
     <row r="519" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A519" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B519" s="25" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="C519" s="25" t="s">
-        <v>387</v>
+        <v>339</v>
       </c>
       <c r="D519" s="18">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E519" s="18" t="s">
         <v>13</v>
@@ -25847,13 +25842,13 @@
         <v>57</v>
       </c>
       <c r="B520" s="25" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="C520" s="25" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D520" s="18">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E520" s="18" t="s">
         <v>13</v>
@@ -25891,13 +25886,13 @@
         <v>57</v>
       </c>
       <c r="B521" s="25" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C521" s="25" t="s">
-        <v>349</v>
+        <v>388</v>
       </c>
       <c r="D521" s="18">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E521" s="18" t="s">
         <v>13</v>
@@ -25932,16 +25927,16 @@
     </row>
     <row r="522" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A522" s="18" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="B522" s="25" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="C522" s="25" t="s">
-        <v>298</v>
+        <v>349</v>
       </c>
       <c r="D522" s="18">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="E522" s="18" t="s">
         <v>13</v>
@@ -25971,21 +25966,21 @@
         <v>22</v>
       </c>
       <c r="N522" s="18" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="523" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A523" s="18" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="B523" s="25" t="s">
-        <v>133</v>
+        <v>48</v>
       </c>
       <c r="C523" s="25" t="s">
-        <v>414</v>
+        <v>298</v>
       </c>
       <c r="D523" s="18">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="E523" s="18" t="s">
         <v>13</v>
@@ -26012,10 +26007,10 @@
         <v>2</v>
       </c>
       <c r="M523" s="18" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="N523" s="18" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="524" spans="1:14" x14ac:dyDescent="0.25">
@@ -26023,13 +26018,13 @@
         <v>98</v>
       </c>
       <c r="B524" s="25" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C524" s="25" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="D524" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E524" s="18" t="s">
         <v>13</v>
@@ -26064,13 +26059,13 @@
     </row>
     <row r="525" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A525" s="18" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B525" s="25" t="s">
-        <v>97</v>
+        <v>138</v>
       </c>
       <c r="C525" s="25" t="s">
-        <v>359</v>
+        <v>424</v>
       </c>
       <c r="D525" s="18">
         <v>1</v>
@@ -26100,7 +26095,7 @@
         <v>2</v>
       </c>
       <c r="M525" s="18" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="N525" s="18" t="s">
         <v>15</v>
@@ -26108,16 +26103,16 @@
     </row>
     <row r="526" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A526" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B526" s="25" t="s">
-        <v>133</v>
+        <v>97</v>
       </c>
       <c r="C526" s="25" t="s">
-        <v>414</v>
+        <v>359</v>
       </c>
       <c r="D526" s="18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E526" s="18" t="s">
         <v>13</v>
@@ -26155,13 +26150,13 @@
         <v>98</v>
       </c>
       <c r="B527" s="25" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C527" s="25" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="D527" s="18">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="E527" s="18" t="s">
         <v>13</v>
@@ -26196,16 +26191,16 @@
     </row>
     <row r="528" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A528" s="18" t="s">
-        <v>189</v>
+        <v>98</v>
       </c>
       <c r="B528" s="25" t="s">
-        <v>204</v>
+        <v>138</v>
       </c>
       <c r="C528" s="25" t="s">
-        <v>474</v>
+        <v>424</v>
       </c>
       <c r="D528" s="18">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="E528" s="18" t="s">
         <v>13</v>
@@ -26240,13 +26235,13 @@
     </row>
     <row r="529" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A529" s="18" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="B529" s="25" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="C529" s="25" t="s">
-        <v>510</v>
+        <v>474</v>
       </c>
       <c r="D529" s="18">
         <v>1</v>
@@ -26284,16 +26279,16 @@
     </row>
     <row r="530" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A530" s="18" t="s">
-        <v>57</v>
+        <v>219</v>
       </c>
       <c r="B530" s="25" t="s">
-        <v>58</v>
+        <v>224</v>
       </c>
       <c r="C530" s="25" t="s">
-        <v>387</v>
+        <v>510</v>
       </c>
       <c r="D530" s="18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E530" s="18" t="s">
         <v>13</v>
@@ -26320,7 +26315,7 @@
         <v>2</v>
       </c>
       <c r="M530" s="18" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="N530" s="18" t="s">
         <v>15</v>
@@ -26331,13 +26326,13 @@
         <v>57</v>
       </c>
       <c r="B531" s="25" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="C531" s="25" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="D531" s="18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E531" s="18" t="s">
         <v>13</v>
@@ -26364,7 +26359,7 @@
         <v>2</v>
       </c>
       <c r="M531" s="18" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="N531" s="18" t="s">
         <v>15</v>
@@ -26375,13 +26370,13 @@
         <v>57</v>
       </c>
       <c r="B532" s="25" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="C532" s="25" t="s">
-        <v>387</v>
+        <v>394</v>
       </c>
       <c r="D532" s="18">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E532" s="18" t="s">
         <v>13</v>
@@ -26408,7 +26403,7 @@
         <v>2</v>
       </c>
       <c r="M532" s="18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N532" s="18" t="s">
         <v>15</v>
@@ -26416,16 +26411,16 @@
     </row>
     <row r="533" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A533" s="18" t="s">
-        <v>560</v>
+        <v>57</v>
       </c>
       <c r="B533" s="25" t="s">
-        <v>561</v>
+        <v>58</v>
       </c>
       <c r="C533" s="25" t="s">
-        <v>562</v>
+        <v>387</v>
       </c>
       <c r="D533" s="18">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E533" s="18" t="s">
         <v>13</v>
@@ -26450,6 +26445,12 @@
       </c>
       <c r="L533" s="18">
         <v>2</v>
+      </c>
+      <c r="M533" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="N533" s="18" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="534" spans="1:14" x14ac:dyDescent="0.25">
@@ -26457,13 +26458,13 @@
         <v>560</v>
       </c>
       <c r="B534" s="25" t="s">
-        <v>568</v>
+        <v>561</v>
       </c>
       <c r="C534" s="25" t="s">
-        <v>571</v>
+        <v>562</v>
       </c>
       <c r="D534" s="18">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E534" s="18" t="s">
         <v>13</v>
@@ -26495,13 +26496,13 @@
         <v>560</v>
       </c>
       <c r="B535" s="25" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="C535" s="25" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="D535" s="18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E535" s="18" t="s">
         <v>13</v>
@@ -26536,10 +26537,10 @@
         <v>574</v>
       </c>
       <c r="C536" s="25" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D536" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E536" s="18" t="s">
         <v>13</v>
@@ -26567,17 +26568,17 @@
       </c>
     </row>
     <row r="537" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A537" s="26" t="s">
+      <c r="A537" s="18" t="s">
         <v>560</v>
       </c>
       <c r="B537" s="25" t="s">
         <v>574</v>
       </c>
       <c r="C537" s="25" t="s">
-        <v>623</v>
+        <v>576</v>
       </c>
       <c r="D537" s="18">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="E537" s="18" t="s">
         <v>13</v>
@@ -26605,17 +26606,17 @@
       </c>
     </row>
     <row r="538" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A538" s="18" t="s">
+      <c r="A538" s="26" t="s">
         <v>560</v>
       </c>
       <c r="B538" s="25" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="C538" s="25" t="s">
-        <v>579</v>
+        <v>623</v>
       </c>
       <c r="D538" s="18">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="E538" s="18" t="s">
         <v>13</v>
@@ -26650,10 +26651,10 @@
         <v>578</v>
       </c>
       <c r="C539" s="25" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D539" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E539" s="18" t="s">
         <v>13</v>
@@ -26681,14 +26682,14 @@
       </c>
     </row>
     <row r="540" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A540" s="26" t="s">
+      <c r="A540" s="18" t="s">
         <v>560</v>
       </c>
       <c r="B540" s="25" t="s">
-        <v>588</v>
+        <v>578</v>
       </c>
       <c r="C540" s="25" t="s">
-        <v>592</v>
+        <v>580</v>
       </c>
       <c r="D540" s="18">
         <v>1</v>
@@ -26723,10 +26724,10 @@
         <v>560</v>
       </c>
       <c r="B541" s="25" t="s">
-        <v>598</v>
+        <v>588</v>
       </c>
       <c r="C541" s="25" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
       <c r="D541" s="18">
         <v>1</v>
@@ -26764,10 +26765,10 @@
         <v>598</v>
       </c>
       <c r="C542" s="25" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D542" s="18">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E542" s="18" t="s">
         <v>13</v>
@@ -26799,13 +26800,13 @@
         <v>560</v>
       </c>
       <c r="B543" s="25" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="C543" s="25" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="D543" s="18">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E543" s="18" t="s">
         <v>13</v>
@@ -26840,10 +26841,10 @@
         <v>601</v>
       </c>
       <c r="C544" s="25" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D544" s="18">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E544" s="18" t="s">
         <v>13</v>
@@ -26875,13 +26876,13 @@
         <v>560</v>
       </c>
       <c r="B545" s="25" t="s">
-        <v>612</v>
+        <v>601</v>
       </c>
       <c r="C545" s="25" t="s">
-        <v>611</v>
+        <v>603</v>
       </c>
       <c r="D545" s="18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E545" s="18" t="s">
         <v>13</v>
@@ -26916,10 +26917,10 @@
         <v>612</v>
       </c>
       <c r="C546" s="25" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="D546" s="18">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E546" s="18" t="s">
         <v>13</v>
@@ -26951,13 +26952,13 @@
         <v>560</v>
       </c>
       <c r="B547" s="25" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="C547" s="25" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D547" s="18">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E547" s="18" t="s">
         <v>13</v>
@@ -26992,10 +26993,10 @@
         <v>615</v>
       </c>
       <c r="C548" s="25" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="D548" s="18">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E548" s="18" t="s">
         <v>13</v>
@@ -27027,13 +27028,13 @@
         <v>560</v>
       </c>
       <c r="B549" s="25" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="C549" s="25" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="D549" s="18">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E549" s="18" t="s">
         <v>13</v>
@@ -27065,10 +27066,10 @@
         <v>560</v>
       </c>
       <c r="B550" s="25" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="C550" s="25" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="D550" s="18">
         <v>3</v>
@@ -27103,13 +27104,13 @@
         <v>560</v>
       </c>
       <c r="B551" s="25" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="C551" s="25" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="D551" s="18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E551" s="18" t="s">
         <v>13</v>
@@ -27144,10 +27145,10 @@
         <v>624</v>
       </c>
       <c r="C552" s="25" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D552" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E552" s="18" t="s">
         <v>13</v>
@@ -27182,10 +27183,10 @@
         <v>624</v>
       </c>
       <c r="C553" s="25" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D553" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E553" s="18" t="s">
         <v>13</v>
@@ -27217,13 +27218,13 @@
         <v>560</v>
       </c>
       <c r="B554" s="25" t="s">
-        <v>633</v>
+        <v>624</v>
       </c>
       <c r="C554" s="25" t="s">
-        <v>634</v>
+        <v>627</v>
       </c>
       <c r="D554" s="18">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E554" s="18" t="s">
         <v>13</v>
@@ -27255,13 +27256,13 @@
         <v>560</v>
       </c>
       <c r="B555" s="25" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="C555" s="25" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="D555" s="18">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="E555" s="18" t="s">
         <v>13</v>
@@ -27296,10 +27297,10 @@
         <v>639</v>
       </c>
       <c r="C556" s="25" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="D556" s="18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E556" s="18" t="s">
         <v>13</v>
@@ -27331,10 +27332,10 @@
         <v>560</v>
       </c>
       <c r="B557" s="25" t="s">
-        <v>647</v>
+        <v>639</v>
       </c>
       <c r="C557" s="25" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="D557" s="18">
         <v>1</v>
@@ -27372,10 +27373,10 @@
         <v>647</v>
       </c>
       <c r="C558" s="25" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="D558" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E558" s="18" t="s">
         <v>13</v>
@@ -27403,17 +27404,17 @@
       </c>
     </row>
     <row r="559" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A559" s="20" t="s">
-        <v>208</v>
+      <c r="A559" s="26" t="s">
+        <v>560</v>
       </c>
       <c r="B559" s="25" t="s">
-        <v>661</v>
+        <v>647</v>
       </c>
       <c r="C559" s="25" t="s">
-        <v>662</v>
-      </c>
-      <c r="D559" s="24">
-        <v>5</v>
+        <v>651</v>
+      </c>
+      <c r="D559" s="18">
+        <v>2</v>
       </c>
       <c r="E559" s="18" t="s">
         <v>13</v>
@@ -27436,7 +27437,7 @@
       <c r="K559" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="L559" s="23">
+      <c r="L559" s="18">
         <v>2</v>
       </c>
     </row>
@@ -27448,10 +27449,10 @@
         <v>661</v>
       </c>
       <c r="C560" s="25" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D560" s="24">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E560" s="18" t="s">
         <v>13</v>
@@ -27483,10 +27484,10 @@
         <v>208</v>
       </c>
       <c r="B561" s="25" t="s">
-        <v>689</v>
+        <v>661</v>
       </c>
       <c r="C561" s="25" t="s">
-        <v>692</v>
+        <v>663</v>
       </c>
       <c r="D561" s="24">
         <v>1</v>
@@ -27521,10 +27522,10 @@
         <v>208</v>
       </c>
       <c r="B562" s="25" t="s">
-        <v>701</v>
+        <v>689</v>
       </c>
       <c r="C562" s="25" t="s">
-        <v>710</v>
+        <v>692</v>
       </c>
       <c r="D562" s="24">
         <v>1</v>
@@ -27555,17 +27556,17 @@
       </c>
     </row>
     <row r="563" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A563" s="18" t="s">
-        <v>37</v>
+      <c r="A563" s="20" t="s">
+        <v>208</v>
       </c>
       <c r="B563" s="25" t="s">
-        <v>38</v>
+        <v>701</v>
       </c>
       <c r="C563" s="25" t="s">
-        <v>310</v>
-      </c>
-      <c r="D563" s="26">
-        <v>5</v>
+        <v>710</v>
+      </c>
+      <c r="D563" s="24">
+        <v>1</v>
       </c>
       <c r="E563" s="18" t="s">
         <v>13</v>
@@ -27580,22 +27581,16 @@
         <v>770</v>
       </c>
       <c r="I563" s="30">
-        <v>51.246899999999997</v>
+        <v>51.244660000000003</v>
       </c>
       <c r="J563" s="30">
-        <v>-80.681020000000004</v>
+        <v>-80.677670000000006</v>
       </c>
       <c r="K563" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="L563" s="18">
-        <v>3</v>
-      </c>
-      <c r="M563" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="N563" s="18" t="s">
-        <v>12</v>
+      <c r="L563" s="23">
+        <v>2</v>
       </c>
     </row>
     <row r="564" spans="1:14" x14ac:dyDescent="0.25">
@@ -27606,10 +27601,10 @@
         <v>38</v>
       </c>
       <c r="C564" s="25" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="D564" s="26">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E564" s="18" t="s">
         <v>13</v>
@@ -27644,16 +27639,16 @@
     </row>
     <row r="565" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A565" s="18" t="s">
-        <v>159</v>
+        <v>37</v>
       </c>
       <c r="B565" s="25" t="s">
-        <v>160</v>
+        <v>38</v>
       </c>
       <c r="C565" s="25" t="s">
-        <v>437</v>
-      </c>
-      <c r="D565" s="18">
-        <v>2</v>
+        <v>316</v>
+      </c>
+      <c r="D565" s="26">
+        <v>1</v>
       </c>
       <c r="E565" s="18" t="s">
         <v>13</v>
@@ -27688,16 +27683,16 @@
     </row>
     <row r="566" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A566" s="18" t="s">
-        <v>185</v>
+        <v>159</v>
       </c>
       <c r="B566" s="25" t="s">
-        <v>186</v>
+        <v>160</v>
       </c>
       <c r="C566" s="25" t="s">
-        <v>452</v>
+        <v>437</v>
       </c>
       <c r="D566" s="18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E566" s="18" t="s">
         <v>13</v>
@@ -27732,16 +27727,16 @@
     </row>
     <row r="567" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A567" s="18" t="s">
-        <v>219</v>
+        <v>185</v>
       </c>
       <c r="B567" s="25" t="s">
-        <v>223</v>
+        <v>186</v>
       </c>
       <c r="C567" s="25" t="s">
-        <v>481</v>
+        <v>452</v>
       </c>
       <c r="D567" s="18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E567" s="18" t="s">
         <v>13</v>
@@ -27768,7 +27763,7 @@
         <v>3</v>
       </c>
       <c r="M567" s="18" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="N567" s="18" t="s">
         <v>12</v>
@@ -27779,10 +27774,10 @@
         <v>219</v>
       </c>
       <c r="B568" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C568" s="25" t="s">
-        <v>509</v>
+        <v>481</v>
       </c>
       <c r="D568" s="18">
         <v>1</v>
@@ -27820,16 +27815,16 @@
     </row>
     <row r="569" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A569" s="18" t="s">
-        <v>37</v>
+        <v>219</v>
       </c>
       <c r="B569" s="25" t="s">
-        <v>38</v>
+        <v>224</v>
       </c>
       <c r="C569" s="25" t="s">
-        <v>310</v>
-      </c>
-      <c r="D569" s="26">
-        <v>5</v>
+        <v>509</v>
+      </c>
+      <c r="D569" s="18">
+        <v>1</v>
       </c>
       <c r="E569" s="18" t="s">
         <v>13</v>
@@ -27856,7 +27851,7 @@
         <v>3</v>
       </c>
       <c r="M569" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N569" s="18" t="s">
         <v>12</v>
@@ -27864,16 +27859,16 @@
     </row>
     <row r="570" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A570" s="18" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="B570" s="25" t="s">
-        <v>99</v>
+        <v>38</v>
       </c>
       <c r="C570" s="25" t="s">
-        <v>401</v>
-      </c>
-      <c r="D570" s="18">
-        <v>2</v>
+        <v>310</v>
+      </c>
+      <c r="D570" s="26">
+        <v>5</v>
       </c>
       <c r="E570" s="18" t="s">
         <v>13</v>
@@ -27911,13 +27906,13 @@
         <v>98</v>
       </c>
       <c r="B571" s="25" t="s">
-        <v>137</v>
+        <v>99</v>
       </c>
       <c r="C571" s="25" t="s">
-        <v>418</v>
+        <v>401</v>
       </c>
       <c r="D571" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E571" s="18" t="s">
         <v>13</v>
@@ -27955,10 +27950,10 @@
         <v>98</v>
       </c>
       <c r="B572" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C572" s="25" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D572" s="18">
         <v>1</v>
@@ -28002,7 +27997,7 @@
         <v>138</v>
       </c>
       <c r="C573" s="25" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="D573" s="18">
         <v>1</v>
@@ -28043,10 +28038,10 @@
         <v>98</v>
       </c>
       <c r="B574" s="25" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C574" s="25" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D574" s="18">
         <v>1</v>
@@ -28090,7 +28085,7 @@
         <v>144</v>
       </c>
       <c r="C575" s="25" t="s">
-        <v>376</v>
+        <v>427</v>
       </c>
       <c r="D575" s="18">
         <v>1</v>
@@ -28128,13 +28123,13 @@
     </row>
     <row r="576" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A576" s="18" t="s">
-        <v>149</v>
+        <v>98</v>
       </c>
       <c r="B576" s="25" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C576" s="25" t="s">
-        <v>430</v>
+        <v>376</v>
       </c>
       <c r="D576" s="18">
         <v>1</v>
@@ -28172,13 +28167,13 @@
     </row>
     <row r="577" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A577" s="18" t="s">
-        <v>185</v>
+        <v>149</v>
       </c>
       <c r="B577" s="25" t="s">
-        <v>186</v>
+        <v>151</v>
       </c>
       <c r="C577" s="25" t="s">
-        <v>453</v>
+        <v>430</v>
       </c>
       <c r="D577" s="18">
         <v>1</v>
@@ -28219,10 +28214,10 @@
         <v>185</v>
       </c>
       <c r="B578" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C578" s="25" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D578" s="18">
         <v>1</v>
@@ -28260,13 +28255,13 @@
     </row>
     <row r="579" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A579" s="18" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B579" s="25" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C579" s="25" t="s">
-        <v>466</v>
+        <v>454</v>
       </c>
       <c r="D579" s="18">
         <v>1</v>
@@ -28304,16 +28299,16 @@
     </row>
     <row r="580" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A580" s="18" t="s">
-        <v>227</v>
+        <v>189</v>
       </c>
       <c r="B580" s="25" t="s">
-        <v>252</v>
+        <v>194</v>
       </c>
       <c r="C580" s="25" t="s">
-        <v>530</v>
+        <v>466</v>
       </c>
       <c r="D580" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E580" s="18" t="s">
         <v>13</v>
@@ -28354,10 +28349,10 @@
         <v>252</v>
       </c>
       <c r="C581" s="25" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D581" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E581" s="18" t="s">
         <v>13</v>
@@ -28392,13 +28387,13 @@
     </row>
     <row r="582" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A582" s="18" t="s">
-        <v>98</v>
+        <v>227</v>
       </c>
       <c r="B582" s="25" t="s">
-        <v>138</v>
+        <v>252</v>
       </c>
       <c r="C582" s="25" t="s">
-        <v>424</v>
+        <v>531</v>
       </c>
       <c r="D582" s="18">
         <v>1</v>
@@ -28428,21 +28423,21 @@
         <v>3</v>
       </c>
       <c r="M582" s="18" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="N582" s="18" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="583" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A583" s="18" t="s">
-        <v>189</v>
+        <v>98</v>
       </c>
       <c r="B583" s="25" t="s">
-        <v>193</v>
+        <v>138</v>
       </c>
       <c r="C583" s="25" t="s">
-        <v>464</v>
+        <v>424</v>
       </c>
       <c r="D583" s="18">
         <v>1</v>
@@ -28480,13 +28475,13 @@
     </row>
     <row r="584" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A584" s="18" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="B584" s="25" t="s">
-        <v>223</v>
+        <v>193</v>
       </c>
       <c r="C584" s="25" t="s">
-        <v>481</v>
+        <v>464</v>
       </c>
       <c r="D584" s="18">
         <v>1</v>
@@ -28527,10 +28522,10 @@
         <v>219</v>
       </c>
       <c r="B585" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C585" s="25" t="s">
-        <v>494</v>
+        <v>481</v>
       </c>
       <c r="D585" s="18">
         <v>1</v>
@@ -28568,16 +28563,16 @@
     </row>
     <row r="586" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A586" s="18" t="s">
-        <v>98</v>
+        <v>219</v>
       </c>
       <c r="B586" s="25" t="s">
-        <v>138</v>
+        <v>224</v>
       </c>
       <c r="C586" s="25" t="s">
-        <v>424</v>
+        <v>494</v>
       </c>
       <c r="D586" s="18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E586" s="18" t="s">
         <v>13</v>
@@ -28604,7 +28599,7 @@
         <v>3</v>
       </c>
       <c r="M586" s="18" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="N586" s="18" t="s">
         <v>15</v>
@@ -28612,16 +28607,16 @@
     </row>
     <row r="587" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A587" s="18" t="s">
-        <v>219</v>
+        <v>98</v>
       </c>
       <c r="B587" s="25" t="s">
-        <v>223</v>
+        <v>138</v>
       </c>
       <c r="C587" s="25" t="s">
-        <v>479</v>
+        <v>424</v>
       </c>
       <c r="D587" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E587" s="18" t="s">
         <v>13</v>
@@ -28662,7 +28657,7 @@
         <v>223</v>
       </c>
       <c r="C588" s="25" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
       <c r="D588" s="18">
         <v>1</v>
@@ -28700,13 +28695,13 @@
     </row>
     <row r="589" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A589" s="18" t="s">
-        <v>98</v>
+        <v>219</v>
       </c>
       <c r="B589" s="25" t="s">
-        <v>138</v>
+        <v>223</v>
       </c>
       <c r="C589" s="25" t="s">
-        <v>424</v>
+        <v>488</v>
       </c>
       <c r="D589" s="18">
         <v>1</v>
@@ -28736,7 +28731,7 @@
         <v>3</v>
       </c>
       <c r="M589" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N589" s="18" t="s">
         <v>15</v>
@@ -28744,13 +28739,13 @@
     </row>
     <row r="590" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A590" s="18" t="s">
-        <v>219</v>
+        <v>98</v>
       </c>
       <c r="B590" s="25" t="s">
-        <v>223</v>
+        <v>138</v>
       </c>
       <c r="C590" s="25" t="s">
-        <v>481</v>
+        <v>424</v>
       </c>
       <c r="D590" s="18">
         <v>1</v>
@@ -28794,7 +28789,7 @@
         <v>223</v>
       </c>
       <c r="C591" s="25" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="D591" s="18">
         <v>1</v>
@@ -28838,10 +28833,10 @@
         <v>223</v>
       </c>
       <c r="C592" s="25" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="D592" s="18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E592" s="18" t="s">
         <v>13</v>
@@ -28876,16 +28871,16 @@
     </row>
     <row r="593" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A593" s="18" t="s">
-        <v>57</v>
+        <v>219</v>
       </c>
       <c r="B593" s="25" t="s">
-        <v>58</v>
+        <v>223</v>
       </c>
       <c r="C593" s="25" t="s">
-        <v>387</v>
+        <v>488</v>
       </c>
       <c r="D593" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E593" s="18" t="s">
         <v>13</v>
@@ -28912,7 +28907,7 @@
         <v>3</v>
       </c>
       <c r="M593" s="18" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="N593" s="18" t="s">
         <v>15</v>
@@ -28929,7 +28924,7 @@
         <v>387</v>
       </c>
       <c r="D594" s="18">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E594" s="18" t="s">
         <v>13</v>
@@ -28956,7 +28951,7 @@
         <v>3</v>
       </c>
       <c r="M594" s="18" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="N594" s="18" t="s">
         <v>15</v>
@@ -28973,7 +28968,7 @@
         <v>387</v>
       </c>
       <c r="D595" s="18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E595" s="18" t="s">
         <v>13</v>
@@ -29000,7 +28995,7 @@
         <v>3</v>
       </c>
       <c r="M595" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N595" s="18" t="s">
         <v>15</v>
@@ -29008,13 +29003,13 @@
     </row>
     <row r="596" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A596" s="18" t="s">
-        <v>560</v>
+        <v>57</v>
       </c>
       <c r="B596" s="25" t="s">
-        <v>561</v>
+        <v>58</v>
       </c>
       <c r="C596" s="25" t="s">
-        <v>562</v>
+        <v>387</v>
       </c>
       <c r="D596" s="18">
         <v>2</v>
@@ -29042,6 +29037,12 @@
       </c>
       <c r="L596" s="18">
         <v>3</v>
+      </c>
+      <c r="M596" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="N596" s="18" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="597" spans="1:14" x14ac:dyDescent="0.25">
@@ -29049,13 +29050,13 @@
         <v>560</v>
       </c>
       <c r="B597" s="25" t="s">
-        <v>574</v>
+        <v>561</v>
       </c>
       <c r="C597" s="25" t="s">
-        <v>575</v>
+        <v>562</v>
       </c>
       <c r="D597" s="18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E597" s="18" t="s">
         <v>13</v>
@@ -29090,10 +29091,10 @@
         <v>574</v>
       </c>
       <c r="C598" s="25" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D598" s="18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E598" s="18" t="s">
         <v>13</v>
@@ -29121,17 +29122,17 @@
       </c>
     </row>
     <row r="599" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A599" s="26" t="s">
+      <c r="A599" s="18" t="s">
         <v>560</v>
       </c>
       <c r="B599" s="25" t="s">
         <v>574</v>
       </c>
       <c r="C599" s="25" t="s">
-        <v>623</v>
+        <v>576</v>
       </c>
       <c r="D599" s="18">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="E599" s="18" t="s">
         <v>13</v>
@@ -29163,13 +29164,13 @@
         <v>560</v>
       </c>
       <c r="B600" s="25" t="s">
-        <v>601</v>
+        <v>574</v>
       </c>
       <c r="C600" s="25" t="s">
-        <v>602</v>
+        <v>623</v>
       </c>
       <c r="D600" s="18">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="E600" s="18" t="s">
         <v>13</v>
@@ -29201,13 +29202,13 @@
         <v>560</v>
       </c>
       <c r="B601" s="25" t="s">
-        <v>612</v>
+        <v>601</v>
       </c>
       <c r="C601" s="25" t="s">
-        <v>611</v>
+        <v>602</v>
       </c>
       <c r="D601" s="18">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E601" s="18" t="s">
         <v>13</v>
@@ -29239,13 +29240,13 @@
         <v>560</v>
       </c>
       <c r="B602" s="25" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="C602" s="25" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="D602" s="18">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E602" s="18" t="s">
         <v>13</v>
@@ -29277,13 +29278,13 @@
         <v>560</v>
       </c>
       <c r="B603" s="25" t="s">
-        <v>624</v>
+        <v>615</v>
       </c>
       <c r="C603" s="25" t="s">
-        <v>625</v>
+        <v>616</v>
       </c>
       <c r="D603" s="18">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E603" s="18" t="s">
         <v>13</v>
@@ -29318,10 +29319,10 @@
         <v>624</v>
       </c>
       <c r="C604" s="25" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D604" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E604" s="18" t="s">
         <v>13</v>
@@ -29353,13 +29354,13 @@
         <v>560</v>
       </c>
       <c r="B605" s="25" t="s">
-        <v>639</v>
+        <v>624</v>
       </c>
       <c r="C605" s="25" t="s">
-        <v>640</v>
+        <v>626</v>
       </c>
       <c r="D605" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E605" s="18" t="s">
         <v>13</v>
@@ -29394,10 +29395,10 @@
         <v>639</v>
       </c>
       <c r="C606" s="25" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D606" s="18">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E606" s="18" t="s">
         <v>13</v>
@@ -29432,10 +29433,10 @@
         <v>639</v>
       </c>
       <c r="C607" s="25" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="D607" s="18">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E607" s="18" t="s">
         <v>13</v>
@@ -29467,13 +29468,13 @@
         <v>560</v>
       </c>
       <c r="B608" s="25" t="s">
-        <v>647</v>
+        <v>639</v>
       </c>
       <c r="C608" s="25" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="D608" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E608" s="18" t="s">
         <v>13</v>
@@ -29508,7 +29509,7 @@
         <v>647</v>
       </c>
       <c r="C609" s="25" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="D609" s="18">
         <v>2</v>
@@ -29539,17 +29540,17 @@
       </c>
     </row>
     <row r="610" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A610" s="20" t="s">
-        <v>208</v>
+      <c r="A610" s="26" t="s">
+        <v>560</v>
       </c>
       <c r="B610" s="25" t="s">
-        <v>661</v>
+        <v>647</v>
       </c>
       <c r="C610" s="25" t="s">
-        <v>662</v>
-      </c>
-      <c r="D610" s="24">
-        <v>12</v>
+        <v>651</v>
+      </c>
+      <c r="D610" s="18">
+        <v>2</v>
       </c>
       <c r="E610" s="18" t="s">
         <v>13</v>
@@ -29572,7 +29573,7 @@
       <c r="K610" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="L610" s="23">
+      <c r="L610" s="18">
         <v>3</v>
       </c>
     </row>
@@ -29581,13 +29582,13 @@
         <v>208</v>
       </c>
       <c r="B611" s="25" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="C611" s="25" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="D611" s="24">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E611" s="18" t="s">
         <v>13</v>
@@ -29622,10 +29623,10 @@
         <v>664</v>
       </c>
       <c r="C612" s="25" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="D612" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E612" s="18" t="s">
         <v>13</v>
@@ -29657,13 +29658,13 @@
         <v>208</v>
       </c>
       <c r="B613" s="25" t="s">
-        <v>672</v>
+        <v>664</v>
       </c>
       <c r="C613" s="25" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="D613" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E613" s="18" t="s">
         <v>13</v>
@@ -29695,13 +29696,13 @@
         <v>208</v>
       </c>
       <c r="B614" s="25" t="s">
-        <v>689</v>
+        <v>672</v>
       </c>
       <c r="C614" s="25" t="s">
-        <v>691</v>
+        <v>673</v>
       </c>
       <c r="D614" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E614" s="18" t="s">
         <v>13</v>
@@ -29729,17 +29730,17 @@
       </c>
     </row>
     <row r="615" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A615" s="26" t="s">
-        <v>560</v>
+      <c r="A615" s="20" t="s">
+        <v>208</v>
       </c>
       <c r="B615" s="25" t="s">
-        <v>615</v>
+        <v>689</v>
       </c>
       <c r="C615" s="25" t="s">
-        <v>616</v>
-      </c>
-      <c r="D615" s="18">
-        <v>8</v>
+        <v>691</v>
+      </c>
+      <c r="D615" s="24">
+        <v>1</v>
       </c>
       <c r="E615" s="18" t="s">
         <v>13</v>
@@ -29754,16 +29755,16 @@
         <v>770</v>
       </c>
       <c r="I615" s="30">
-        <v>51.246220000000001</v>
+        <v>51.246899999999997</v>
       </c>
       <c r="J615" s="30">
-        <v>-80.672809999999998</v>
+        <v>-80.681020000000004</v>
       </c>
       <c r="K615" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="L615" s="18">
-        <v>1</v>
+      <c r="L615" s="23">
+        <v>3</v>
       </c>
     </row>
     <row r="616" spans="1:14" x14ac:dyDescent="0.25">
@@ -64367,6 +64368,8 @@
   </sheetData>
   <sortState ref="A2:N1449">
     <sortCondition ref="E2:E1449"/>
+    <sortCondition ref="K2:K1449"/>
+    <sortCondition ref="L2:L1449"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>